<commit_message>
Use values of 0 for NOx and OC GWP (which were previously negative)
</commit_message>
<xml_diff>
--- a/InputData/fuels/GbPbT/GWP by Pollutant by Timeframe.xlsx
+++ b/InputData/fuels/GbPbT/GWP by Pollutant by Timeframe.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="21328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="25128"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\deept\OneDrive\Desktop\Input Data for India 2.0\fuels\GbPbT\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mmahajan\Documents\eps-india-highgdp\InputData\fuels\GbPbT\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{47013458-D16F-4D0A-B163-995E9006FE93}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FF4F95AD-277D-45B0-8E26-768CFA730736}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="17640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="About" sheetId="1" r:id="rId1"/>
@@ -22,7 +22,11 @@
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
         <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -30,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="42">
   <si>
     <t>Source:</t>
   </si>
@@ -153,6 +157,9 @@
   </si>
   <si>
     <t>updated for India from the IPCC source, using "South Asia" rows in the tables.</t>
+  </si>
+  <si>
+    <t>We have customized the India EPS to use values of 0 for Nox and OC.</t>
   </si>
 </sst>
 </file>
@@ -568,24 +575,24 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B13"/>
+  <dimension ref="A1:B15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E14" sqref="E14"/>
+      <selection activeCell="A16" sqref="A16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="2" max="2" width="14.140625" customWidth="1"/>
-    <col min="3" max="3" width="41.42578125" customWidth="1"/>
+    <col min="2" max="2" width="14.1796875" customWidth="1"/>
+    <col min="3" max="3" width="41.453125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A3" s="1" t="s">
         <v>0</v>
       </c>
@@ -593,44 +600,49 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
       <c r="B4" s="2">
         <v>2013</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
       <c r="B5" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.35">
       <c r="B6" s="3" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.35">
       <c r="B7" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A9" s="1" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
         <v>26</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A15" t="s">
+        <v>41</v>
       </c>
     </row>
   </sheetData>
@@ -650,13 +662,13 @@
       <selection activeCell="D14" sqref="D14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="2" max="3" width="18.5703125" customWidth="1"/>
+    <col min="2" max="3" width="18.54296875" customWidth="1"/>
     <col min="4" max="4" width="80" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A1" s="5"/>
       <c r="B1" s="6" t="s">
         <v>12</v>
@@ -668,7 +680,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>4</v>
       </c>
@@ -682,7 +694,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>5</v>
       </c>
@@ -696,7 +708,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>16</v>
       </c>
@@ -710,7 +722,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>6</v>
       </c>
@@ -724,7 +736,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>7</v>
       </c>
@@ -738,7 +750,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>8</v>
       </c>
@@ -752,7 +764,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>9</v>
       </c>
@@ -766,7 +778,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
         <v>21</v>
       </c>
@@ -780,7 +792,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
         <v>22</v>
       </c>
@@ -794,7 +806,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
         <v>10</v>
       </c>
@@ -808,7 +820,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
         <v>11</v>
       </c>
@@ -822,7 +834,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
         <v>17</v>
       </c>
@@ -836,12 +848,12 @@
         <v>18</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.35">
       <c r="D14" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.35">
       <c r="D15" t="s">
         <v>20</v>
       </c>
@@ -859,17 +871,17 @@
   <dimension ref="A1:C13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C10" sqref="C10"/>
+      <selection activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="13.42578125" customWidth="1"/>
-    <col min="2" max="2" width="17.42578125" customWidth="1"/>
-    <col min="3" max="3" width="20.28515625" customWidth="1"/>
+    <col min="1" max="1" width="13.453125" customWidth="1"/>
+    <col min="2" max="2" width="17.453125" customWidth="1"/>
+    <col min="3" max="3" width="20.26953125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>33</v>
       </c>
@@ -880,7 +892,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A2" s="1" t="str">
         <f>Data!A2</f>
         <v>CO2</v>
@@ -894,7 +906,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A3" s="1" t="str">
         <f>Data!A3</f>
         <v>VOC</v>
@@ -908,7 +920,7 @@
         <v>8.8000000000000007</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A4" s="1" t="str">
         <f>Data!A4</f>
         <v>CO</v>
@@ -922,21 +934,19 @@
         <v>1.8</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A5" s="1" t="str">
         <f>Data!A5</f>
         <v>NOx</v>
       </c>
       <c r="B5" s="4">
-        <f>Data!B5</f>
-        <v>-40.700000000000003</v>
+        <v>0</v>
       </c>
       <c r="C5" s="4">
-        <f>Data!C5</f>
-        <v>-25.3</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A6" s="1" t="str">
         <f>Data!A6</f>
         <v>PM10</v>
@@ -950,7 +960,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A7" s="1" t="str">
         <f>Data!A7</f>
         <v>PM25</v>
@@ -964,7 +974,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A8" s="1" t="str">
         <f>Data!A8</f>
         <v>SOx</v>
@@ -978,7 +988,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A9" s="1" t="str">
         <f>Data!A9</f>
         <v>BC</v>
@@ -992,21 +1002,19 @@
         <v>345</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A10" s="1" t="str">
         <f>Data!A10</f>
         <v>OC</v>
       </c>
       <c r="B10" s="4">
-        <f>Data!B10</f>
-        <v>-160</v>
+        <v>0</v>
       </c>
       <c r="C10" s="4">
-        <f>Data!C10</f>
-        <v>-46</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A11" s="1" t="str">
         <f>Data!A11</f>
         <v>CH4</v>
@@ -1020,7 +1028,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A12" s="1" t="str">
         <f>Data!A12</f>
         <v>N2O</v>
@@ -1034,7 +1042,7 @@
         <v>265</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A13" s="1" t="str">
         <f>Data!A13</f>
         <v>F gases</v>

</xml_diff>